<commit_message>
bi: update oncho stop forms
</commit_message>
<xml_diff>
--- a/ONCHO/Impact Assessments/Burundi/bi_oncho_prestop_2_202307_questions.xlsx
+++ b/ONCHO/Impact Assessments/Burundi/bi_oncho_prestop_2_202307_questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Impact Assessments\Burundi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E89A28-AA11-44A2-BB08-F6ECBD6B44AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E53A3C3-700D-4B30-9CA0-BA6F6BE935C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="120">
   <si>
     <t>form_title</t>
   </si>
@@ -86,9 +86,6 @@
     <t>hint::French</t>
   </si>
   <si>
-    <t>Entrer l'identifiant de l'enregistreur</t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
@@ -140,12 +137,6 @@
     <t>regex(.,'^[0-9]{2}$') and . &gt; 9 and . &lt; 1000</t>
   </si>
   <si>
-    <t>Sélectionner un arrondissement</t>
-  </si>
-  <si>
-    <t>note</t>
-  </si>
-  <si>
     <t>barcode</t>
   </si>
   <si>
@@ -155,9 +146,6 @@
     <t>select_one yes_no</t>
   </si>
   <si>
-    <t>Le participant a-t-il donné son consentement?</t>
-  </si>
-  <si>
     <t>sex</t>
   </si>
   <si>
@@ -182,21 +170,12 @@
     <t>Refuse de repondre</t>
   </si>
   <si>
-    <t>2) Sélectionner un village</t>
-  </si>
-  <si>
-    <t>4) Numéro de maison</t>
-  </si>
-  <si>
     <t>5) Numéro d'identification du participant</t>
   </si>
   <si>
     <t>6) Quel est le sexe du participant?</t>
   </si>
   <si>
-    <t>9) Depuis combien d'années vivez-vous / votre enfant vit-il dans le village ?</t>
-  </si>
-  <si>
     <t>frequence</t>
   </si>
   <si>
@@ -242,9 +221,6 @@
     <t>Note additionelle</t>
   </si>
   <si>
-    <t>string</t>
-  </si>
-  <si>
     <t>p_RecorderID</t>
   </si>
   <si>
@@ -254,18 +230,9 @@
     <t>p_District</t>
   </si>
   <si>
-    <t>p_site_name</t>
-  </si>
-  <si>
     <t>p_consent</t>
   </si>
   <si>
-    <t>p_inf_gen</t>
-  </si>
-  <si>
-    <t>p_num_maison</t>
-  </si>
-  <si>
     <t>p_barecode_id</t>
   </si>
   <si>
@@ -284,15 +251,6 @@
     <t>p_EndTime</t>
   </si>
   <si>
-    <t>${p_consent} = 'Oui'</t>
-  </si>
-  <si>
-    <t>${p_region} = region_list</t>
-  </si>
-  <si>
-    <t>${p_District} = district_list</t>
-  </si>
-  <si>
     <t>Scanner</t>
   </si>
   <si>
@@ -311,18 +269,9 @@
     <t>p_manual_id</t>
   </si>
   <si>
-    <t>${p_consent} = 'Oui' and ${p_id_type} = 'Scanner'</t>
-  </si>
-  <si>
-    <t>${p_consent} = 'Oui' and ${p_id_type} = 'Manuel'</t>
-  </si>
-  <si>
     <t>Manuel</t>
   </si>
   <si>
-    <t>INFORMATIONS GENERALES</t>
-  </si>
-  <si>
     <t>tranch_age</t>
   </si>
   <si>
@@ -344,16 +293,112 @@
     <t>9 ans</t>
   </si>
   <si>
-    <t>bi_oncho_prestop_2_202307_questions</t>
-  </si>
-  <si>
-    <t>(2023 Juillet) ONCHO pre Stop - 2. Questionnaire individuel</t>
-  </si>
-  <si>
     <t>p_age_yrs</t>
   </si>
   <si>
     <t>7) Sélectionner la tranche d'âge du participant</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>p_date</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Code enquêteur</t>
+  </si>
+  <si>
+    <t>Nom et Prénom du chef d'quipe</t>
+  </si>
+  <si>
+    <t>r_chef_equipe</t>
+  </si>
+  <si>
+    <t>Sélectionner une province</t>
+  </si>
+  <si>
+    <t>Sélectionner un district</t>
+  </si>
+  <si>
+    <t>Sélectionner un centre de santé</t>
+  </si>
+  <si>
+    <t>Entrer le nom du village/Colline</t>
+  </si>
+  <si>
+    <t>p_commune</t>
+  </si>
+  <si>
+    <t>p_centre_sante</t>
+  </si>
+  <si>
+    <t>p_Cluster_Name</t>
+  </si>
+  <si>
+    <t>Participant /Son titulaire  a donné son consentement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9) Séjour du participant dans le village </t>
+  </si>
+  <si>
+    <t>. &gt;= ${p_age_yrs}</t>
+  </si>
+  <si>
+    <t>Le séjour ne doit pas être supérieur à l'âge</t>
+  </si>
+  <si>
+    <t>begin repeat</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Ajouter un nouveau participant</t>
+  </si>
+  <si>
+    <t>Ajouter</t>
+  </si>
+  <si>
+    <t>Ne pas ajouter</t>
+  </si>
+  <si>
+    <t>add_part</t>
+  </si>
+  <si>
+    <t>select_one add_part</t>
+  </si>
+  <si>
+    <t>p_add_participant</t>
+  </si>
+  <si>
+    <t>${p_consent} = 'Oui' and ${p_add_participant} = 'Ajouter'</t>
+  </si>
+  <si>
+    <t>${p_consent} = 'Oui' and ${p_id_type} = 'Scanner' and ${p_add_participant} = 'Ajouter'</t>
+  </si>
+  <si>
+    <t>${p_consent} = 'Oui' and ${p_id_type} = 'Manuel' and ${p_add_participant} = 'Ajouter'</t>
+  </si>
+  <si>
+    <t>end repeat</t>
+  </si>
+  <si>
+    <t>${p_add_participant} = 'Ajouter'</t>
+  </si>
+  <si>
+    <t>(2023 Juillet) ONCHO pre Stop - 2. Questionnaire individuel V2</t>
+  </si>
+  <si>
+    <t>bi_oncho_prestop_2_202307_questions_v2</t>
+  </si>
+  <si>
+    <t>p_pris_dbs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insérer la prise du sang sur  DBS  </t>
   </si>
 </sst>
 </file>
@@ -516,9 +561,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -555,6 +597,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -845,13 +890,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15:XFD18"/>
+      <selection pane="bottomRight" activeCell="F19" sqref="F19:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -890,7 +935,7 @@
         <v>6</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>7</v>
@@ -908,400 +953,510 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>25</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="D2" s="9"/>
       <c r="E2" s="10"/>
-      <c r="F2" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>31</v>
-      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="9"/>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
       <c r="J2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="9"/>
+        <v>89</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="E3" s="10"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="9"/>
+      <c r="F3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="16"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="10"/>
       <c r="I4" s="10"/>
-      <c r="J4" s="6" t="s">
-        <v>24</v>
+      <c r="J4" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="K4" s="10"/>
-      <c r="L4" s="11" t="s">
-        <v>82</v>
-      </c>
+      <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="6"/>
+        <v>20</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="10"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="6" t="s">
-        <v>24</v>
+      <c r="J5" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="K5" s="10"/>
-      <c r="L5" s="11" t="s">
-        <v>83</v>
-      </c>
+      <c r="L5" s="10"/>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="6"/>
+        <v>20</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="16"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
       <c r="G6" s="13"/>
-      <c r="H6" s="10"/>
+      <c r="H6" s="8"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="6" t="s">
-        <v>24</v>
+      <c r="J6" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
+      <c r="L6" s="8"/>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="I7" s="26"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
+      <c r="A7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="10"/>
+      <c r="L7" s="8"/>
     </row>
     <row r="8" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="6"/>
+        <v>20</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="22" t="s">
-        <v>81</v>
-      </c>
+      <c r="H8" s="8"/>
       <c r="I8" s="10"/>
-      <c r="J8" s="6" t="s">
-        <v>24</v>
+      <c r="J8" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
+      <c r="L8" s="8"/>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="22" t="s">
-        <v>81</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17"/>
       <c r="I9" s="10"/>
-      <c r="J9" s="6" t="s">
-        <v>24</v>
+      <c r="J9" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-    </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-    </row>
-    <row r="11" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="L9" s="8"/>
+    </row>
+    <row r="10" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+    </row>
+    <row r="11" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>89</v>
+        <v>109</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>110</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="10"/>
       <c r="F11" s="6"/>
       <c r="G11" s="13"/>
-      <c r="H11" s="22" t="s">
-        <v>91</v>
-      </c>
+      <c r="H11" s="21"/>
       <c r="I11" s="10"/>
       <c r="J11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
     </row>
     <row r="12" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>76</v>
+        <v>34</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>63</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="10"/>
       <c r="F12" s="6"/>
       <c r="G12" s="13"/>
-      <c r="H12" s="22" t="s">
-        <v>81</v>
+      <c r="H12" s="10" t="s">
+        <v>115</v>
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
     </row>
-    <row r="13" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>103</v>
+        <v>72</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>73</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="10"/>
       <c r="F13" s="6"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="22" t="s">
-        <v>81</v>
+      <c r="H13" s="21" t="s">
+        <v>111</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
     </row>
-    <row r="14" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>77</v>
+        <v>32</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>64</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="10"/>
       <c r="F14" s="6"/>
       <c r="G14" s="13"/>
-      <c r="H14" s="22" t="s">
-        <v>81</v>
+      <c r="H14" s="21" t="s">
+        <v>112</v>
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
     </row>
-    <row r="15" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>78</v>
+        <v>20</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>75</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="10"/>
       <c r="F15" s="6"/>
       <c r="G15" s="13"/>
-      <c r="H15" s="10"/>
+      <c r="H15" s="21" t="s">
+        <v>113</v>
+      </c>
       <c r="I15" s="10"/>
-      <c r="J15" s="6"/>
+      <c r="J15" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
     </row>
-    <row r="16" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="9"/>
+    <row r="16" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="D16" s="9"/>
       <c r="E16" s="10"/>
       <c r="F16" s="6"/>
       <c r="G16" s="13"/>
-      <c r="H16" s="10"/>
+      <c r="H16" s="21" t="s">
+        <v>111</v>
+      </c>
       <c r="I16" s="10"/>
-      <c r="J16" s="6"/>
+      <c r="J16" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
     </row>
-    <row r="17" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="I17" s="10"/>
+      <c r="J17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+    </row>
+    <row r="18" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="I18" s="10"/>
+      <c r="J18" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+    </row>
+    <row r="19" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="I19" s="10"/>
+      <c r="J19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+    </row>
+    <row r="20" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+    </row>
+    <row r="21" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" s="15"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+    </row>
+    <row r="22" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+    </row>
+    <row r="23" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-    </row>
-    <row r="18" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
+      <c r="B23" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+    </row>
+    <row r="24" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1314,8 +1469,8 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24:A28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1336,552 +1491,564 @@
         <v>13</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="C2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+    </row>
+    <row r="4" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+    </row>
+    <row r="5" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+    </row>
+    <row r="6" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+    </row>
+    <row r="7" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-    </row>
-    <row r="3" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-    </row>
-    <row r="4" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+    </row>
+    <row r="8" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="C8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+    </row>
+    <row r="9" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-    </row>
-    <row r="5" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="11" t="s">
+      <c r="B9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-    </row>
-    <row r="6" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-    </row>
-    <row r="7" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-    </row>
-    <row r="8" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-    </row>
-    <row r="9" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="11" t="s">
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+    </row>
+    <row r="10" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C10" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+    </row>
+    <row r="11" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-    </row>
-    <row r="10" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="B11" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+    </row>
+    <row r="12" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+    </row>
+    <row r="13" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+    </row>
+    <row r="14" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+    </row>
+    <row r="15" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+    </row>
+    <row r="16" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="C16" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+    </row>
+    <row r="17" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C17" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-    </row>
-    <row r="11" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="11" t="s">
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+    </row>
+    <row r="18" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C18" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-    </row>
-    <row r="12" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="11" t="s">
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+    </row>
+    <row r="19" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+    </row>
+    <row r="20" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C20" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-    </row>
-    <row r="13" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-    </row>
-    <row r="14" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" s="11" t="s">
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+    </row>
+    <row r="21" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-    </row>
-    <row r="15" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" s="11" t="s">
+      <c r="B21" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C21" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-    </row>
-    <row r="16" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-    </row>
-    <row r="17" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-    </row>
-    <row r="18" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-    </row>
-    <row r="19" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-    </row>
-    <row r="20" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-    </row>
-    <row r="21" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-    </row>
-    <row r="22" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+    </row>
+    <row r="22" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-    </row>
-    <row r="23" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+    </row>
+    <row r="23" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-    </row>
-    <row r="24" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+    </row>
+    <row r="24" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="B24" s="11">
         <v>5</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-    </row>
-    <row r="25" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+    </row>
+    <row r="25" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="B25" s="11">
         <v>6</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
+        <v>80</v>
+      </c>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="B26" s="11">
         <v>7</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="19"/>
+        <v>81</v>
+      </c>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="18"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="B27" s="11">
         <v>8</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="19"/>
+        <v>82</v>
+      </c>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="18"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="B28" s="11">
         <v>9</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="19"/>
+        <v>83</v>
+      </c>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="18"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="19"/>
+      <c r="A29" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="18"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="19"/>
+      <c r="A30" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="18"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="18"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="18"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="18"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="18"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="18"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="18"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="18"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="18"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="18"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="18"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="18"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="18"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="18"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="18"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="18"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="18"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="18"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="11"/>
       <c r="C48" s="11"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="18"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A49:B59">
@@ -1897,8 +2064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1918,21 +2085,21 @@
         <v>12</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>